<commit_message>
Added Demos for Week 10
</commit_message>
<xml_diff>
--- a/Docs/Nisharg Soni-G2.xlsx
+++ b/Docs/Nisharg Soni-G2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RKIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NishargSoni-458\RKIT_TRAINING\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D0A4A-6000-4867-A1AF-407E9D9E444C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE98DB9-3557-45E1-8EEB-F5A6FE752EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="836" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="836" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="12" r:id="rId1"/>
@@ -29,15 +29,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -50,10 +41,19 @@
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C31472CF-B693-43E5-8460-8E6FC3EC18EF}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Add date on which respected topic is completed  </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="239">
   <si>
     <t>#</t>
   </si>
@@ -778,9 +778,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -1286,11 +1283,11 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1457,22 +1454,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF7AA6-4C8D-4242-B5C6-D93B1FDDA835}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1787,19 +1784,19 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="1"/>
-    <col min="7" max="7" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2204,19 +2201,19 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2824,19 +2821,19 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3241,19 +3238,19 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3568,22 +3565,22 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="1"/>
-    <col min="7" max="7" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3943,21 +3940,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1E0EC-E2AF-45C4-9952-AF78B78D30CC}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4009,7 +4008,10 @@
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="G2" s="11">
+        <v>46027</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4029,7 +4031,10 @@
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="G3" s="11">
+        <v>46028</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4049,7 +4054,10 @@
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>236</v>
+      </c>
+      <c r="G4" s="11">
+        <v>46029</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4069,7 +4077,10 @@
         <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>236</v>
+      </c>
+      <c r="G5" s="11">
+        <v>46030</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4089,7 +4100,10 @@
         <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>236</v>
+      </c>
+      <c r="G6" s="11">
+        <v>46030</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4109,7 +4123,10 @@
         <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>236</v>
+      </c>
+      <c r="G7" s="11">
+        <v>46030</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4158,14 +4175,14 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4327,15 +4344,15 @@
       <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4527,12 +4544,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3C32926E4737E47B27DDAA5D371959A" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="10250be6089a57ac4e60aefa3d8c7247">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a7998c3e-7f65-4586-b9f5-db7168bdbc10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f71cd174da29f72f20168de9339b0a7a" ns2:_="">
     <xsd:import namespace="a7998c3e-7f65-4586-b9f5-db7168bdbc10"/>
@@ -4670,16 +4696,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55EF8721-4A61-4D2C-A16B-F3152A60B6FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56DCEFB2-4877-4926-B462-8A1B0C5C05F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4688,7 +4713,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA151C35-975C-4B59-AE26-DA6BD662A7F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4704,12 +4729,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55EF8721-4A61-4D2C-A16B-F3152A60B6FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>